<commit_message>
Ready to move to vps
</commit_message>
<xml_diff>
--- a/pepeCards/pepeCards.xlsx
+++ b/pepeCards/pepeCards.xlsx
@@ -668,7 +668,13 @@
         <v>502</v>
       </c>
       <c r="R5" t="str">
-        <v>No</v>
+        <v>Yes</v>
+      </c>
+      <c r="S5" t="str">
+        <v>0xD6eA1686B523EcC32742771d659065E73eC3eE46</v>
+      </c>
+      <c r="T5" t="str">
+        <v>127.0.0.1</v>
       </c>
     </row>
     <row r="6">

</xml_diff>